<commit_message>
Thiet lap ngay dat hang du kien, sua loi gui mail
</commit_message>
<xml_diff>
--- a/storage/app/public/thong_tin_phieu_dat_hang.xlsx
+++ b/storage/app/public/thong_tin_phieu_dat_hang.xlsx
@@ -36,9 +36,6 @@
     <t xml:space="preserve">Mã phiếu: </t>
   </si>
   <si>
-    <t>Thông tin phiếu đặt hàng</t>
-  </si>
-  <si>
     <t>Ngày 28 tháng 10 năm 2024</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>Cảm ơn bạn đã hợp tác với chúng tôi!</t>
   </si>
   <si>
-    <t>Trân trọng, TC Shop Company</t>
-  </si>
-  <si>
     <t>Địa chỉ:</t>
   </si>
   <si>
@@ -76,6 +70,12 @@
   </si>
   <si>
     <t>Thành tiền (VND)</t>
+  </si>
+  <si>
+    <t>Ngày nhận hàng dự kiến:</t>
+  </si>
+  <si>
+    <t>THÔNG TIN PHIẾU ĐẶT HÀNG</t>
   </si>
 </sst>
 </file>
@@ -203,10 +203,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -556,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:E21"/>
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -573,49 +573,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="A2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
@@ -625,125 +625,127 @@
     <row r="7" spans="1:5" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="10" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="7" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>1</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="C15" s="14">
         <v>1</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11">
+      <c r="D15" s="11">
         <v>3</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E15" s="12">
         <v>30000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+    </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
+      <c r="A20" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A21:E21"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="2321" orientation="portrait" r:id="rId1"/>

</xml_diff>